<commit_message>
#13, penambahan halaman manajemen user, custom template
</commit_message>
<xml_diff>
--- a/backend/web/template/tpl_rkpd.xlsx
+++ b/backend/web/template/tpl_rkpd.xlsx
@@ -10,6 +10,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
@@ -264,17 +265,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="centerContinuous" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -310,6 +305,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -626,12 +624,12 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="18.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="63.7109375" style="1" customWidth="1"/>
     <col min="3" max="3" width="40.42578125" style="1" customWidth="1"/>
     <col min="4" max="5" width="19.85546875" style="1" customWidth="1"/>
@@ -641,141 +639,144 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="21">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
     </row>
     <row r="2" spans="1:8" ht="21">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
     </row>
     <row r="3" spans="1:8" ht="21">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
     </row>
     <row r="4" spans="1:8" ht="15.75" thickBot="1"/>
     <row r="5" spans="1:8" ht="45" customHeight="1" thickTop="1">
-      <c r="A5" s="17" t="s">
+      <c r="A5" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="19" t="s">
+      <c r="C5" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="16" t="s">
+      <c r="D5" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="16"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="19" t="s">
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="H5" s="21"/>
+      <c r="H5" s="20"/>
     </row>
     <row r="6" spans="1:8" ht="30">
-      <c r="A6" s="18"/>
-      <c r="B6" s="20"/>
-      <c r="C6" s="20"/>
-      <c r="D6" s="5" t="s">
+      <c r="A6" s="17"/>
+      <c r="B6" s="19"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="F6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="G6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="H6" s="8" t="s">
+      <c r="H6" s="6" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="F7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="G7" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="H7" s="10" t="s">
+      <c r="H7" s="8" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="20.25" customHeight="1">
-      <c r="A8" s="11"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="12"/>
+      <c r="A8" s="9"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="10"/>
     </row>
     <row r="9" spans="1:8" ht="20.25" customHeight="1">
-      <c r="A9" s="11"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="12"/>
+      <c r="A9" s="9"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="10"/>
     </row>
     <row r="10" spans="1:8" ht="20.25" customHeight="1" thickBot="1">
-      <c r="A10" s="13"/>
-      <c r="B10" s="14"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="15"/>
+      <c r="A10" s="11"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="13"/>
     </row>
     <row r="11" spans="1:8" ht="15.75" thickTop="1"/>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="8">
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="A3:H3"/>
     <mergeCell ref="D5:F5"/>
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="B5:B6"/>
@@ -809,4 +810,18 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>